<commit_message>
Palo fijo colors and text changes
</commit_message>
<xml_diff>
--- a/TableGrid.xlsx
+++ b/TableGrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_NewDudo\Dudo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C80554-478A-4C22-B76A-75CE8C5D5CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1C3A89-D2EB-4DD8-BCF7-08F722C0B574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="24" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="6" sheetId="14" r:id="rId6"/>
     <sheet name="7" sheetId="13" r:id="rId7"/>
     <sheet name="8" sheetId="12" r:id="rId8"/>
+    <sheet name="3 (2)" sheetId="26" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -161,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -178,7 +179,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6CF5762-392D-43A8-B0FA-89F60659BC54}">
   <dimension ref="A2:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1348,8 +1348,6 @@
       <c r="C9" s="4"/>
       <c r="F9" s="5"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
       <c r="J9" s="5"/>
       <c r="K9" s="4"/>
       <c r="N9" s="5"/>
@@ -1557,7 +1555,6 @@
       </c>
       <c r="B9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="14"/>
       <c r="H9" s="5"/>
       <c r="L9" s="5"/>
     </row>
@@ -1765,7 +1762,6 @@
       </c>
       <c r="B9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="14"/>
       <c r="H9" s="5"/>
       <c r="L9" s="5"/>
     </row>
@@ -1973,7 +1969,6 @@
       </c>
       <c r="B9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="14"/>
       <c r="H9" s="5"/>
       <c r="L9" s="5"/>
     </row>
@@ -2058,4 +2053,193 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C12316-84E1-4324-BF31-90BAF10FDE2A}">
+  <dimension ref="A2:M14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="9">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9">
+        <v>3</v>
+      </c>
+      <c r="F2" s="9">
+        <v>4</v>
+      </c>
+      <c r="G2" s="9">
+        <v>5</v>
+      </c>
+      <c r="H2" s="9">
+        <v>6</v>
+      </c>
+      <c r="I2" s="9">
+        <v>7</v>
+      </c>
+      <c r="J2" s="9">
+        <v>8</v>
+      </c>
+      <c r="K2" s="9">
+        <v>9</v>
+      </c>
+      <c r="L2" s="9">
+        <v>10</v>
+      </c>
+      <c r="M2" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="F5" s="5"/>
+      <c r="I5" s="4"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="8"/>
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="3"/>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="I9" s="5"/>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="8"/>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="M13" s="5"/>
+    </row>
+    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>11</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>